<commit_message>
replace with 20 pin cp2102
</commit_message>
<xml_diff>
--- a/CAD/BT832 BOM.xlsx
+++ b/CAD/BT832 BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="112">
   <si>
     <t>Part</t>
   </si>
@@ -31,6 +31,21 @@
     <t>Notes</t>
   </si>
   <si>
+    <t>US Mouser prices</t>
+  </si>
+  <si>
+    <t>5 Assembled Turnkey Quote (China prices)</t>
+  </si>
+  <si>
+    <t>5sets</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
     <t>BT832A</t>
   </si>
   <si>
@@ -40,13 +55,32 @@
     <t>BLE + CortexM4/M4F</t>
   </si>
   <si>
+    <t>The higher priced chips are cheaper from the manufacturer</t>
+  </si>
+  <si>
+    <t>3.75 ea on Fanstel</t>
+  </si>
+  <si>
+    <t>7-10work days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CP2102N-A02-GQFN20R
+</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>USB-UART</t>
+  </si>
+  <si>
+    <t>CP2102-GMR QFN-28</t>
+  </si>
+  <si>
     <t>CP2102</t>
   </si>
   <si>
-    <t>IC1</t>
-  </si>
-  <si>
-    <t>USB-UART</t>
+    <t>Incorrect PN</t>
   </si>
   <si>
     <t>DX4R005JJ2R1800</t>
@@ -76,6 +110,9 @@
     <t>3.3V LDO</t>
   </si>
   <si>
+    <t>LP5907MFX-3.3/NOPB</t>
+  </si>
+  <si>
     <t>X2</t>
   </si>
   <si>
@@ -91,6 +128,9 @@
     <t>8.192MHz XTAL</t>
   </si>
   <si>
+    <t>LFXTAL061486Reel 7-10work days ok or not</t>
+  </si>
+  <si>
     <t>GCM1555C1H100JA16D</t>
   </si>
   <si>
@@ -145,6 +185,9 @@
     <t>220uF Cap</t>
   </si>
   <si>
+    <t>offer part 220nF</t>
+  </si>
+  <si>
     <t>C0603C104J4REC7411</t>
   </si>
   <si>
@@ -154,6 +197,9 @@
     <t>100uF Cap</t>
   </si>
   <si>
+    <t>offer part 100nF 7-10work days</t>
+  </si>
+  <si>
     <t>GRM155R60J106ME05D</t>
   </si>
   <si>
@@ -223,15 +269,24 @@
     <t>Use Ebay bulk or aliexpress</t>
   </si>
   <si>
+    <t>J1 485-1769 5PCS $1.05/PCS 7-10WORK DAYS</t>
+  </si>
+  <si>
+    <t>MCP73831T-5ACI/MC</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>Battery regulator</t>
+  </si>
+  <si>
+    <t>MCP73831T-2ACI/OT SOT23-5 ok or not</t>
+  </si>
+  <si>
     <t>MCP73831T</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>Battery regulator</t>
-  </si>
-  <si>
     <t>BCM857BS-7-F</t>
   </si>
   <si>
@@ -241,15 +296,18 @@
     <t>Bipolar Transistor</t>
   </si>
   <si>
+    <t>B5817WS-TP</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Schottkey Diode</t>
+  </si>
+  <si>
     <t>B5817WS</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>Schottkey Diode</t>
-  </si>
-  <si>
     <t>BAT1000-7-F</t>
   </si>
   <si>
@@ -278,13 +336,28 @@
   </si>
   <si>
     <t>Switch On-Off</t>
+  </si>
+  <si>
+    <t>2-3 weeks</t>
+  </si>
+  <si>
+    <t>Totals:</t>
+  </si>
+  <si>
+    <t>$311 w/ assembly</t>
+  </si>
+  <si>
+    <t>$30 Shipping</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -294,17 +367,39 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <color theme="1"/>
-      <name val="Inherit"/>
+      <sz val="8.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
       <color rgb="FF1155CC"/>
     </font>
     <font>
+      <sz val="8.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <u/>
+      <color rgb="FF1155CC"/>
+      <name val="Inherit"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8.0"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8.0"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
@@ -320,7 +415,19 @@
     </font>
     <font>
       <u/>
+      <sz val="8.0"/>
+      <color rgb="FF0070BB"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
       <sz val="9.0"/>
+      <color rgb="FF0070BB"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8.0"/>
       <color rgb="FF0070BB"/>
       <name val="Arial"/>
     </font>
@@ -331,15 +438,35 @@
       <name val="Times New Roman"/>
     </font>
     <font>
-      <name val="Inherit"/>
+      <u/>
+      <sz val="8.0"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8.0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -360,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -368,35 +495,78 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -613,10 +783,14 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.57"/>
+    <col customWidth="1" min="1" max="1" width="22.29"/>
     <col customWidth="1" min="2" max="2" width="24.14"/>
     <col customWidth="1" min="3" max="3" width="7.86"/>
     <col customWidth="1" min="5" max="5" width="24.71"/>
+    <col customWidth="1" min="8" max="8" width="16.29"/>
+    <col customWidth="1" min="13" max="13" width="16.86"/>
+    <col customWidth="1" min="14" max="14" width="37.57"/>
+    <col customWidth="1" min="17" max="17" width="20.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -638,443 +812,1230 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="J1" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="K1" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="L1" s="1">
+        <v>1000.0</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
+      <c r="A2" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>1.0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1">
+        <v>7.33</v>
+      </c>
+      <c r="J2" s="1">
+        <v>67.3</v>
+      </c>
+      <c r="K2" s="1">
+        <v>550.0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>3920.0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="6">
+        <v>10.92</v>
+      </c>
+      <c r="P2" s="6">
+        <v>54.6</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1">
         <v>1.0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1.85</v>
+      </c>
+      <c r="J3" s="1">
+        <v>17.6</v>
+      </c>
+      <c r="K3" s="1">
+        <v>155.0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1390.0</v>
+      </c>
+      <c r="O3" s="8">
+        <v>3.99</v>
+      </c>
+      <c r="P3" s="8">
+        <v>19.95</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
+      <c r="A4" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1">
         <v>1.0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="J4" s="1">
+        <v>6.32</v>
+      </c>
+      <c r="K4" s="1">
+        <v>54.9</v>
+      </c>
+      <c r="L4" s="1">
+        <v>386.0</v>
+      </c>
+      <c r="O4" s="6">
+        <v>1.155</v>
+      </c>
+      <c r="P4" s="6">
+        <v>5.775</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
+      <c r="A5" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1">
         <v>1.0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="I5" s="1">
+        <v>8.04</v>
+      </c>
+      <c r="J5" s="1">
+        <v>72.7</v>
+      </c>
+      <c r="K5" s="1">
+        <v>611.0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>4.98</v>
+      </c>
+      <c r="O5" s="6">
+        <v>11.55</v>
+      </c>
+      <c r="P5" s="6">
+        <v>57.75</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1">
         <v>2.0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="J6" s="1">
+        <v>5.37</v>
+      </c>
+      <c r="K6" s="1">
+        <v>37.2</v>
+      </c>
+      <c r="L6" s="1">
+        <v>244.0</v>
+      </c>
+      <c r="O6" s="6">
+        <v>1.05</v>
+      </c>
+      <c r="P6" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R6" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5">
+      <c r="A7" s="13">
         <v>8.30050789E8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1">
         <v>1.0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="J7" s="1">
+        <v>5.67</v>
+      </c>
+      <c r="K7" s="1">
+        <v>50.1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>384.0</v>
+      </c>
+      <c r="O7" s="6">
+        <v>0.945</v>
+      </c>
+      <c r="P7" s="6">
+        <v>4.725</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R7" s="14">
+        <v>8.30050789E8</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1">
         <v>1.0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="6">
+        <v>37</v>
+      </c>
+      <c r="E8" s="15">
         <v>8.30061486E8</v>
       </c>
+      <c r="I8" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="J8" s="1">
+        <v>6.38</v>
+      </c>
+      <c r="K8" s="1">
+        <v>56.4</v>
+      </c>
+      <c r="L8" s="1">
+        <v>432.0</v>
+      </c>
+      <c r="O8" s="6">
+        <v>1.05</v>
+      </c>
+      <c r="P8" s="6">
+        <v>5.25</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="s">
-        <v>26</v>
+      <c r="A9" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1">
         <v>2.0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>29</v>
+        <v>41</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="K9" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="L9" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="O9" s="6">
+        <v>0.053</v>
+      </c>
+      <c r="P9" s="6">
+        <v>0.525</v>
+      </c>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="s">
-        <v>31</v>
+      <c r="A10" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1">
         <v>2.0</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>29</v>
+      <c r="D10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.29</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L10" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="O10" s="6">
+        <v>0.053</v>
+      </c>
+      <c r="P10" s="6">
+        <v>0.525</v>
+      </c>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="s">
-        <v>35</v>
+      <c r="A11" s="19" t="s">
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1">
         <v>1.0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>29</v>
+        <v>50</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="K11" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="O11" s="6">
+        <v>0.105</v>
+      </c>
+      <c r="P11" s="6">
+        <v>0.525</v>
+      </c>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="s">
-        <v>38</v>
+      <c r="A12" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="2">
+        <v>52</v>
+      </c>
+      <c r="C12" s="1">
         <v>6.0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>29</v>
+        <v>53</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="L12" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="O12" s="6">
+        <v>0.105</v>
+      </c>
+      <c r="P12" s="6">
+        <v>3.15</v>
+      </c>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="9" t="s">
-        <v>41</v>
+      <c r="A13" s="21" t="s">
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1">
         <v>1.0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>29</v>
+        <v>56</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="K13" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="L13" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="O13" s="6">
+        <v>0.105</v>
+      </c>
+      <c r="P13" s="6">
+        <v>0.525</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R13" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="9" t="s">
-        <v>44</v>
+      <c r="A14" s="21" t="s">
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1">
         <v>1.0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>29</v>
+        <v>60</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1.12</v>
+      </c>
+      <c r="K14" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="O14" s="6">
+        <v>0.525</v>
+      </c>
+      <c r="P14" s="6">
+        <v>2.625</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="R14" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="s">
-        <v>47</v>
+      <c r="A15" s="19" t="s">
+        <v>62</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C15" s="1">
         <v>1.0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>29</v>
+        <v>64</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1.12</v>
+      </c>
+      <c r="K15" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="L15" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="O15" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="P15" s="6">
+        <v>1.05</v>
+      </c>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="A16" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="1">
         <v>2.0</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>29</v>
+      <c r="D16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="K16" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="L16" s="1">
+        <v>38.0</v>
+      </c>
+      <c r="O16" s="6">
+        <v>0.105</v>
+      </c>
+      <c r="P16" s="6">
+        <v>1.05</v>
+      </c>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="A17" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="1">
         <v>2.0</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>56</v>
+      <c r="D17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="O17" s="6">
+        <v>0.053</v>
+      </c>
+      <c r="P17" s="6">
+        <v>0.525</v>
+      </c>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="A18" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="1">
         <v>2.0</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>56</v>
+      <c r="D18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.14</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L18" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="O18" s="6">
+        <v>0.053</v>
+      </c>
+      <c r="P18" s="6">
+        <v>0.525</v>
+      </c>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="A19" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="1">
         <v>1.0</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>56</v>
+      <c r="D19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="L19" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="O19" s="6">
+        <v>0.053</v>
+      </c>
+      <c r="P19" s="6">
+        <v>0.263</v>
+      </c>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="A20" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="1">
         <v>1.0</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>65</v>
+      <c r="D20" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>56</v>
+        <v>71</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="L20" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="O20" s="6">
+        <v>0.053</v>
+      </c>
+      <c r="P20" s="6">
+        <v>0.263</v>
+      </c>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="S20" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="2">
+        <v>81</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="1">
         <v>1.0</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>68</v>
+      <c r="D21" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>69</v>
+        <v>84</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="J21" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="O21" s="6">
+        <v>1.05</v>
+      </c>
+      <c r="P21" s="6">
+        <v>5.25</v>
+      </c>
+      <c r="Q21" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="R21" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="A22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="1">
         <v>1.0</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>72</v>
+      <c r="D22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="J22" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="K22" s="1">
+        <v>54.6</v>
+      </c>
+      <c r="L22" s="1">
+        <v>540.6</v>
+      </c>
+      <c r="O22" s="6">
+        <v>1.26</v>
+      </c>
+      <c r="P22" s="6">
+        <v>6.3</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="R22" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="S22" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="2">
+      <c r="A23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="1">
         <v>1.0</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>75</v>
+      <c r="D23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="J23" s="1">
+        <v>2.57</v>
+      </c>
+      <c r="K23" s="1">
+        <v>13.6</v>
+      </c>
+      <c r="L23" s="1">
+        <v>61.0</v>
+      </c>
+      <c r="O23" s="6">
+        <v>0.525</v>
+      </c>
+      <c r="P23" s="6">
+        <v>2.625</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="2">
+      <c r="A24" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="1">
         <v>1.0</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F24" s="11"/>
+      <c r="D24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="25"/>
+      <c r="I24" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="J24" s="1">
+        <v>3.34</v>
+      </c>
+      <c r="K24" s="1">
+        <v>19.0</v>
+      </c>
+      <c r="L24" s="1">
+        <v>97.0</v>
+      </c>
+      <c r="O24" s="6">
+        <v>0.105</v>
+      </c>
+      <c r="P24" s="6">
+        <v>0.525</v>
+      </c>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="S24" s="7" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" s="2">
+      <c r="A25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="1">
         <v>2.0</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>81</v>
+      <c r="D25" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>82</v>
+        <v>101</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.57</v>
+      </c>
+      <c r="J25" s="1">
+        <v>4.95</v>
+      </c>
+      <c r="K25" s="1">
+        <v>37.0</v>
+      </c>
+      <c r="L25" s="1">
+        <v>225.0</v>
+      </c>
+      <c r="O25" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="P25" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="2">
+      <c r="A26" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="1">
         <v>2.0</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>85</v>
+      <c r="D26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="J26" s="1">
+        <v>3.22</v>
+      </c>
+      <c r="K26" s="1">
+        <v>25.8</v>
+      </c>
+      <c r="L26" s="1">
+        <v>214.0</v>
+      </c>
+      <c r="O26" s="6">
+        <v>0.735</v>
+      </c>
+      <c r="P26" s="6">
+        <v>7.35</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R26" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="S26" s="7" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="s">
-        <v>86</v>
+      <c r="A27" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="C27" s="1">
         <v>1.0</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>88</v>
+        <v>107</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="J27" s="1">
+        <v>8.37</v>
+      </c>
+      <c r="K27" s="1">
+        <v>66.1</v>
+      </c>
+      <c r="L27" s="1">
+        <v>533.0</v>
+      </c>
+      <c r="O27" s="6">
+        <v>3.15</v>
+      </c>
+      <c r="P27" s="6">
+        <v>15.75</v>
+      </c>
+      <c r="Q27" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" s="26">
+        <f>SUM(C2:C27)</f>
+        <v>39</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I28" s="26">
+        <f t="shared" ref="I28:L28" si="1">SUM(I2:I27)</f>
+        <v>25.71</v>
+      </c>
+      <c r="J28" s="26">
+        <f t="shared" si="1"/>
+        <v>223</v>
+      </c>
+      <c r="K28" s="26">
+        <f t="shared" si="1"/>
+        <v>1776.5</v>
+      </c>
+      <c r="L28" s="26">
+        <f t="shared" si="1"/>
+        <v>8750.58</v>
+      </c>
+      <c r="O28" s="17"/>
+      <c r="P28" s="6">
+        <v>210.0</v>
+      </c>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+    </row>
+    <row r="30">
+      <c r="P30" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="P31" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A6"/>
-    <hyperlink r:id="rId2" ref="A7"/>
-    <hyperlink r:id="rId3" ref="A8"/>
-    <hyperlink r:id="rId4" ref="E8"/>
-    <hyperlink r:id="rId5" ref="A9"/>
-    <hyperlink r:id="rId6" ref="A10"/>
-    <hyperlink r:id="rId7" ref="A11"/>
-    <hyperlink r:id="rId8" ref="A12"/>
-    <hyperlink r:id="rId9" ref="A13"/>
-    <hyperlink r:id="rId10" ref="A14"/>
-    <hyperlink r:id="rId11" ref="A15"/>
-    <hyperlink r:id="rId12" ref="A16"/>
-    <hyperlink r:id="rId13" ref="A17"/>
-    <hyperlink r:id="rId14" ref="A18"/>
-    <hyperlink r:id="rId15" ref="A19"/>
-    <hyperlink r:id="rId16" ref="A20"/>
-    <hyperlink r:id="rId17" ref="A26"/>
+    <hyperlink r:id="rId1" ref="A2"/>
+    <hyperlink r:id="rId2" ref="A3"/>
+    <hyperlink r:id="rId3" ref="A4"/>
+    <hyperlink r:id="rId4" ref="A5"/>
+    <hyperlink r:id="rId5" ref="A6"/>
+    <hyperlink r:id="rId6" ref="R6"/>
+    <hyperlink r:id="rId7" ref="A7"/>
+    <hyperlink r:id="rId8" ref="A8"/>
+    <hyperlink r:id="rId9" ref="E8"/>
+    <hyperlink r:id="rId10" ref="R8"/>
+    <hyperlink r:id="rId11" ref="A9"/>
+    <hyperlink r:id="rId12" ref="R9"/>
+    <hyperlink r:id="rId13" ref="A10"/>
+    <hyperlink r:id="rId14" ref="R10"/>
+    <hyperlink r:id="rId15" ref="A11"/>
+    <hyperlink r:id="rId16" ref="R11"/>
+    <hyperlink r:id="rId17" ref="A12"/>
+    <hyperlink r:id="rId18" ref="R12"/>
+    <hyperlink r:id="rId19" ref="A13"/>
+    <hyperlink r:id="rId20" ref="R13"/>
+    <hyperlink r:id="rId21" ref="A14"/>
+    <hyperlink r:id="rId22" ref="R14"/>
+    <hyperlink r:id="rId23" ref="A15"/>
+    <hyperlink r:id="rId24" ref="R15"/>
+    <hyperlink r:id="rId25" ref="A16"/>
+    <hyperlink r:id="rId26" ref="R16"/>
+    <hyperlink r:id="rId27" ref="A17"/>
+    <hyperlink r:id="rId28" ref="R17"/>
+    <hyperlink r:id="rId29" ref="A18"/>
+    <hyperlink r:id="rId30" ref="R18"/>
+    <hyperlink r:id="rId31" ref="A19"/>
+    <hyperlink r:id="rId32" ref="R19"/>
+    <hyperlink r:id="rId33" ref="A20"/>
+    <hyperlink r:id="rId34" ref="R20"/>
+    <hyperlink r:id="rId35" ref="A21"/>
+    <hyperlink r:id="rId36" ref="A22"/>
+    <hyperlink r:id="rId37" ref="A23"/>
+    <hyperlink r:id="rId38" ref="A24"/>
+    <hyperlink r:id="rId39" ref="A25"/>
+    <hyperlink r:id="rId40" ref="A26"/>
+    <hyperlink r:id="rId41" ref="R26"/>
+    <hyperlink r:id="rId42" ref="A27"/>
   </hyperlinks>
-  <drawing r:id="rId18"/>
+  <drawing r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>